<commit_message>
1,modify airdrop_list file. Delete some useless code. 2,change airdropList code.
</commit_message>
<xml_diff>
--- a/Airdrop/airdrop_list/itc_airdrop_total.xlsx
+++ b/Airdrop/airdrop_list/itc_airdrop_total.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuoapp/Documents/zhoyiyu/GithubAirdrop/Airdrop/airdrop_list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/Project/GithubTokenAirdrop/Airdrop/airdrop_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="440" windowWidth="27740" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="440" windowWidth="27700" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -397,15 +397,10 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="98.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
modify airdropList.js file path
</commit_message>
<xml_diff>
--- a/Airdrop/airdrop_list/itc_airdrop_total.xlsx
+++ b/Airdrop/airdrop_list/itc_airdrop_total.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="440" windowWidth="27700" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="440" windowWidth="27740" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Timestamp</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>0x3d816b62645db347a04e3b3ea7866672471b30b0</t>
+  </si>
+  <si>
+    <t>@Larsblm</t>
+  </si>
+  <si>
+    <t>https://twitter.com/Larsblm/status/959369283116716036</t>
+  </si>
+  <si>
+    <t>0x645a06e738adea003014583f5e42508e6ecbb040</t>
   </si>
 </sst>
 </file>
@@ -394,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -444,11 +453,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>43133.096827175927</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>